<commit_message>
ccdi 2620 - 4 scripts input excels for 4 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC03_CCDI_PHS-Accession-phs003111_Race-Wht_DiagClassSys-ICD_SampAnatSite-Liver.xlsx
+++ b/InputFiles/CCDI/TC03_CCDI_PHS-Accession-phs003111_Race-Wht_DiagClassSys-ICD_SampAnatSite-Liver.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9122D9-0E14-41D1-BF7E-7CAEDC50C60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479C31E3-4375-469D-9EBC-6FD7A4E3E76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>WebExcel</t>
   </si>
@@ -417,12 +417,18 @@
   apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
   apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
   </si>
+  <si>
+    <t>TC03_CCDI_PHS-Accession-phs003111_Race-Wht_DiagClassSys-ICD_SampAnatSite-Liver_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC03_CCDI_PHS-Accession-phs003111_Race-Wht_DiagClassSys-ICD_SampAnatSite-Liver_WebData.xlsx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +456,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -472,10 +484,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -796,7 +809,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,104 +822,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="330" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>